<commit_message>
Updates covid return spec
</commit_message>
<xml_diff>
--- a/specifications/covid/Business intelligence systems - System Development - BI Project - Covid (All) - v1.9.xlsx
+++ b/specifications/covid/Business intelligence systems - System Development - BI Project - Covid (All) - v1.9.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\ShrForms\specifications\covid\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5136989-F2B0-4B9E-8664-4B4822C74D36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCB3D708-F14E-4352-8D30-8AB101A56C50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="799" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="799" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Version Control" sheetId="2" r:id="rId1"/>
@@ -3492,7 +3492,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:E11"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="80" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
@@ -3646,7 +3646,7 @@
         <v>445</v>
       </c>
       <c r="D11" s="65" t="s">
-        <v>22</v>
+        <v>406</v>
       </c>
       <c r="E11" s="66" t="s">
         <v>446</v>
@@ -4041,7 +4041,7 @@
   </sheetPr>
   <dimension ref="A1:AB135"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="8" topLeftCell="C117" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C33" sqref="C33"/>
       <selection pane="topRight" activeCell="C33" sqref="C33"/>

</xml_diff>